<commit_message>
try to plot policy by time map
</commit_message>
<xml_diff>
--- a/CN_Provinces/Yuhang_Pan-CN_lockdown_data.xlsx
+++ b/CN_Provinces/Yuhang_Pan-CN_lockdown_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smileternity/Dropbox/Research/cov2019/cov2019_work/new_workfile_generate/raw_data/regulation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qitianhu/Documents/Research/Explore/COVID-19_sosc/CN_Provinces/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DFBC2FC-DEE3-914E-BF66-0E0361B880E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDD6B6E-802D-174A-A9F9-4C77A7E486C2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="880" yWindow="460" windowWidth="25600" windowHeight="14480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,12 +33,6 @@
     <t>city_name2010</t>
   </si>
   <si>
-    <t>北京|北京</t>
-  </si>
-  <si>
-    <t>天津|天津</t>
-  </si>
-  <si>
     <t>石家庄市</t>
   </si>
   <si>
@@ -111,9 +105,6 @@
     <t>葫芦岛市</t>
   </si>
   <si>
-    <t>上海|上海</t>
-  </si>
-  <si>
     <t>南京市</t>
   </si>
   <si>
@@ -231,9 +222,6 @@
     <t>宜昌市</t>
   </si>
   <si>
-    <t>襄樊市</t>
-  </si>
-  <si>
     <t>鄂州市</t>
   </si>
   <si>
@@ -273,9 +261,6 @@
     <t>防城港市</t>
   </si>
   <si>
-    <t>重慶|重庆</t>
-  </si>
-  <si>
     <t>内江市</t>
   </si>
   <si>
@@ -574,10 +559,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>莱芜市</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Laiwu</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -708,23 +689,41 @@
   <si>
     <t>仙桃市</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>天津市</t>
+  </si>
+  <si>
+    <t>北京市</t>
+  </si>
+  <si>
+    <t>上海市</t>
+  </si>
+  <si>
+    <t>重庆市</t>
+  </si>
+  <si>
+    <t>襄阳市</t>
+  </si>
+  <si>
+    <t>莱芜区</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1040,18 +1039,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="159" workbookViewId="0">
-      <selection activeCell="E68" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="36.5" customWidth="1"/>
     <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1059,567 +1058,567 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>4201</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D2" s="2">
         <v>20200123</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>4202</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D3" s="2">
         <v>20200124</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>4203</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="D4" s="2">
         <v>20200124</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4205</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D5" s="2">
         <v>20200124</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4207</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D6" s="2">
         <v>20200124</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>4208</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D7" s="2">
         <v>20200124</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>4209</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D8" s="2">
         <v>20200124</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>4211</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D9" s="2">
         <v>20200124</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>4212</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="D10" s="2">
         <v>20200124</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>4228</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="D11" s="2">
         <v>20200124</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>1303</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D12" s="2">
         <v>20200125</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>4206</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>68</v>
+        <v>191</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D13" s="2">
         <v>20200126</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>4210</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D14" s="2">
         <v>20200126</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>999997</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D15" s="2">
         <v>20200126</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>1302</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D16" s="2">
         <v>20200128</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>3705</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D17" s="2">
         <v>20200130</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>5000</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>82</v>
+        <v>190</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D18" s="2">
         <v>20200131</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>6401</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="D19" s="2">
         <v>20200131</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>6403</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="D20" s="2">
         <v>20200131</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>3303</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D21" s="2">
         <v>20200202</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>3202</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D22" s="2">
         <v>20200203</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>3708</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D23" s="2">
         <v>20200203</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>2301</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D24" s="2">
         <v>20200204</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>3201</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D25" s="2">
         <v>20200204</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>3203</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D26" s="2">
         <v>20200204</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>3204</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D27" s="2">
         <v>20200204</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>3206</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D28" s="2">
         <v>20200204</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>3301</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D29" s="2">
         <v>20200204</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>3302</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D30" s="2">
         <v>20200204</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>3501</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D31" s="2">
         <v>20200204</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>3602</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D32" s="2">
         <v>20200204</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>3704</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D33" s="2">
         <v>20200204</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>3713</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D34" s="2">
         <v>20200204</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>4101</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D35" s="2">
         <v>20200204</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>4117</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D36" s="2">
         <v>20200204</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>2101</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D37" s="2">
         <v>20200205</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>2102</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D38" s="2">
         <v>20200205</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>2103</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D39" s="2">
         <v>20200205</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>2104</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D40" s="2">
         <v>20200205</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>2105</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D41" s="2">
         <v>20200205</v>
@@ -1627,15 +1626,15 @@
       <c r="F41" s="1"/>
       <c r="G41" s="2"/>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>2106</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D42" s="2">
         <v>20200205</v>
@@ -1643,757 +1642,757 @@
       <c r="F42" s="1"/>
       <c r="G42" s="2"/>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>2107</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D43" s="2">
         <v>20200205</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>2109</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D44" s="2">
         <v>20200205</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>2110</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D45" s="2">
         <v>20200205</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>2111</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D46" s="2">
         <v>20200205</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>2112</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D47" s="2">
         <v>20200205</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>2113</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D48" s="2">
         <v>20200205</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>2114</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D49" s="2">
         <v>20200205</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>3210</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="D50" s="2">
         <v>20200205</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>3401</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D51" s="2">
         <v>20200205</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>3505</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D52" s="2">
         <v>20200205</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>3601</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D53" s="2">
         <v>20200205</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>3701</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D54" s="2">
         <v>20200205</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>3702</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D55" s="2">
         <v>20200205</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>3709</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D56" s="2">
         <v>20200205</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>3711</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D57" s="2">
         <v>20200205</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>3712</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>159</v>
+        <v>192</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D58" s="2">
         <v>20200205</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>4501</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D59" s="2">
         <v>20200205</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>5301</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D60" s="2">
         <v>20200205</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>1200</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>3</v>
+        <v>187</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D61" s="2">
         <v>20200206</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>1301</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D62" s="2">
         <v>20200206</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>3205</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D63" s="2">
         <v>20200206</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>3603</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D64" s="2">
         <v>20200206</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>3604</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D65" s="2">
         <v>20200206</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>3605</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D66" s="2">
         <v>20200206</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>3606</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D67" s="2">
         <v>20200206</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>3607</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D68" s="2">
         <v>20200206</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>3608</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D69" s="2">
         <v>20200206</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>3609</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D70" s="2">
         <v>20200206</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>3610</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D71" s="2">
         <v>20200206</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>3611</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D72" s="2">
         <v>20200206</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>5110</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="D73" s="2">
         <v>20200206</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>5115</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D74" s="2">
         <v>20200206</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>4115</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="D75" s="2">
         <v>20200206</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>4213</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="D76" s="2">
         <v>20200207</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>4401</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D77" s="2">
         <v>20200207</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>4403</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D78" s="2">
         <v>20200208</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>4406</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D79" s="2">
         <v>20200208</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>4506</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="D80" s="2">
         <v>20200208</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>1309</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D81" s="2">
         <v>20200209</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>3406</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D82" s="2">
         <v>20200209</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>1100</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>2</v>
+        <v>188</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D83" s="2">
         <v>20200210</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>3100</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>28</v>
+        <v>189</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D84" s="2">
         <v>20200210</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>1501</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D85" s="2">
         <v>20200213</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>1502</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D86" s="2">
         <v>20200213</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>1503</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D87" s="2">
         <v>20200213</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>1504</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D88" s="2">
         <v>20200213</v>
       </c>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>1505</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D89" s="2">
         <v>20200213</v>
       </c>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>1506</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D90" s="2">
         <v>20200213</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>1507</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D91" s="2">
         <v>20200213</v>
       </c>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>1508</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D92" s="2">
         <v>20200213</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>1509</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D93" s="2">
         <v>20200213</v>
       </c>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>1522</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="D94" s="2">
         <v>20200213</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>1525</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D95" s="2">
         <v>20200213</v>
       </c>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>1529</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D96" s="2">
         <v>20200213</v>

</xml_diff>